<commit_message>
add Oauth test, add: byte-encoded field to test framework
</commit_message>
<xml_diff>
--- a/TestingSpecifications.xlsx
+++ b/TestingSpecifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="4" r:id="rId1"/>
@@ -14,14 +14,14 @@
     <sheet name="Plugin Notification option" sheetId="7" r:id="rId5"/>
     <sheet name="Dailylife" sheetId="1" r:id="rId6"/>
     <sheet name="Circle" sheetId="6" r:id="rId7"/>
-    <sheet name="Account-bind" sheetId="9" r:id="rId8"/>
+    <sheet name="Account-binding" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
   <si>
     <t xml:space="preserve">post a comment, and request comment detail </t>
   </si>
@@ -275,9 +275,6 @@
     <t>invite buddies to a created discussion</t>
   </si>
   <si>
-    <t>Invited buddies accept invitation</t>
-  </si>
-  <si>
     <t>Discussion's offline member does not receive notification when new member join</t>
   </si>
   <si>
@@ -329,34 +326,79 @@
     <t>Discussion message sent using the same request id  from a member is treated as one message</t>
   </si>
   <si>
-    <t>Other discussion members receive discussion info changed notification</t>
-  </si>
-  <si>
     <t>Server returns discussion option when member requests</t>
   </si>
   <si>
     <t>Discussion member can request discussion option</t>
   </si>
   <si>
-    <t>Other discussion member can change discussion info</t>
-  </si>
-  <si>
-    <t>Discussion creator can change discussion info</t>
-  </si>
-  <si>
     <t>Online - Invited buddy receives invitation if invited to discussion</t>
   </si>
   <si>
     <t>account-bind</t>
   </si>
   <si>
-    <t>User requests to bind to an account without parameter, server returns error</t>
-  </si>
-  <si>
-    <t>User requests to bind to an account with valid parameter, server returns bind response</t>
-  </si>
-  <si>
-    <t>User requests to bind to an account with an invalid parameter, server returns error</t>
+    <t xml:space="preserve">User requests to bind to another number with valid parameter, server returns bind response </t>
+  </si>
+  <si>
+    <t>User request list bound accounts</t>
+  </si>
+  <si>
+    <t>Server returns list bound accounts</t>
+  </si>
+  <si>
+    <t>User removes accounts from list bound accounts</t>
+  </si>
+  <si>
+    <t>account-bind-multiple</t>
+  </si>
+  <si>
+    <t>account-bind-contact-update</t>
+  </si>
+  <si>
+    <t>When member in discussion does not ack a discussion message, they will receive it again</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User requests to update contact, </t>
+  </si>
+  <si>
+    <t>User requests to add contacts to his bound accounts, when this contact is already bound, friend request is sent</t>
+  </si>
+  <si>
+    <t>User requests to add contacts to his bound accounts, when another account has his contact on their contact list, a buddy recommendation is returned</t>
+  </si>
+  <si>
+    <t>User requests to add contacts to his bound accounts, when the other account has him on contact list already, both are added as friend.</t>
+  </si>
+  <si>
+    <t>User requests to bind to an invalid phone number with valid param, server returns error (invalid param)</t>
+  </si>
+  <si>
+    <t>User requests to bind to a valid phone number with valid parameter, server returns bind response</t>
+  </si>
+  <si>
+    <t>User requests to bind to a valid phone number without parameter, server returns verification-required error</t>
+  </si>
+  <si>
+    <t>User requests to bind to a valid phone number with an invalid parameter, server returns verification error</t>
+  </si>
+  <si>
+    <t>User requests to bind to a valid phone number with valid parameter again, server returns expired login error</t>
+  </si>
+  <si>
+    <t>Discussion members can change discussion info</t>
+  </si>
+  <si>
+    <t>Invited buddies accept invitation, receives notification</t>
+  </si>
+  <si>
+    <t>Interleaved messages from different members in the discussion are received in order they are sent</t>
+  </si>
+  <si>
+    <t>Online discussion members receive discussion info changed notification</t>
+  </si>
+  <si>
+    <t>Offline discussion members does not receive discussion info changed notification</t>
   </si>
 </sst>
 </file>
@@ -767,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,21 +880,23 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="1">
-        <f>SUM(B3:H3)</f>
-        <v>0</v>
+        <f>SUM(B3:K3)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -867,13 +911,21 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="4"/>
+      <c r="H4" s="5">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L30" si="0">SUM(B4:H4)</f>
-        <v>1</v>
+        <f t="shared" ref="L4:L30" si="0">SUM(B4:K4)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -899,25 +951,40 @@
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="1"/>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -927,32 +994,41 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="1"/>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="4">
-        <v>1</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="I8" s="4">
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <v>1</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
       <c r="L8" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="B9" s="4">
         <v>1</v>
@@ -961,19 +1037,27 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="I9" s="4">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
       <c r="L9" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -981,15 +1065,20 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="4">
+        <v>1</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="1"/>
+      <c r="L10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
@@ -1010,9 +1099,11 @@
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1024,74 +1115,95 @@
       <c r="K12" s="4"/>
       <c r="L12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="4">
+        <v>1</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="1">
-        <f t="shared" ref="L14" si="1">SUM(B14:H14)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>1</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="1"/>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4">
         <v>1</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1101,18 +1213,20 @@
       <c r="K16" s="4"/>
       <c r="L16" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4">
         <v>1</v>
       </c>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1122,18 +1236,20 @@
       <c r="K17" s="4"/>
       <c r="L17" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4">
         <v>1</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1143,18 +1259,20 @@
       <c r="K18" s="4"/>
       <c r="L18" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4">
         <v>1</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1164,18 +1282,18 @@
       <c r="K19" s="4"/>
       <c r="L19" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1188,15 +1306,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4">
         <v>1</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1206,18 +1326,20 @@
       <c r="K21" s="4"/>
       <c r="L21" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4">
         <v>1</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1227,16 +1349,20 @@
       <c r="K22" s="4"/>
       <c r="L22" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1246,17 +1372,19 @@
       <c r="K23" s="4"/>
       <c r="L23" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
@@ -1264,18 +1392,20 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="1">
-        <f t="shared" ref="L24" si="2">SUM(B24:H24)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
@@ -1284,12 +1414,12 @@
       <c r="K25" s="4"/>
       <c r="L25" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1298,17 +1428,21 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
+      <c r="I26" s="4">
+        <v>1</v>
+      </c>
+      <c r="J26" s="4">
+        <v>1</v>
+      </c>
       <c r="K26" s="4"/>
       <c r="L26" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1317,17 +1451,23 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="I27" s="4">
+        <v>1</v>
+      </c>
+      <c r="J27" s="4">
+        <v>1</v>
+      </c>
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
       <c r="L27" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1338,44 +1478,58 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4">
+        <v>1</v>
+      </c>
       <c r="L28" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="I29" s="4">
+        <v>1</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4">
+        <v>1</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1383,36 +1537,45 @@
         <v>34</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" ref="B31:H31" si="3">SUM(B3:B30)</f>
+        <f>SUM(B3:B30)</f>
+        <v>7</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" ref="C31:K31" si="1">SUM(C3:C30)</f>
+        <v>8</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C31" s="1">
-        <f t="shared" si="3"/>
+      <c r="F31" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="D31" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="J31" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
       <c r="L31" s="1"/>
     </row>
   </sheetData>
@@ -2803,10 +2966,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,13 +2991,17 @@
       <c r="H1" s="3"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2843,9 +3010,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -2857,50 +3024,60 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="1">
-        <f>SUM(B3:H3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I3:I15" si="0">SUM(B3:H3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="4"/>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I25" si="0">SUM(B4:H4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2908,13 +3085,19 @@
       <c r="H6" s="4"/>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -2922,13 +3105,17 @@
       <c r="H7" s="4"/>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -2936,13 +3123,19 @@
       <c r="H8" s="4"/>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -2950,13 +3143,19 @@
       <c r="H9" s="4"/>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -2964,13 +3163,19 @@
       <c r="H10" s="4"/>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -2978,238 +3183,114 @@
       <c r="H11" s="4"/>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4">
+        <v>1</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="1">
-        <f t="shared" ref="B26:H26" si="1">SUM(B3:B25)</f>
-        <v>3</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:H16" si="1">SUM(C2:C15)</f>
+        <v>8</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D26" s="1">
+      <c r="F16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E26" s="1">
+      <c r="G16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F26" s="1">
+      <c r="H16" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G26" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="1"/>
+      <c r="I16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
finish feature tests - version 1.0
</commit_message>
<xml_diff>
--- a/TestingSpecifications.xlsx
+++ b/TestingSpecifications.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="4" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Dailylife" sheetId="1" r:id="rId6"/>
     <sheet name="Circle" sheetId="6" r:id="rId7"/>
     <sheet name="Account-binding" sheetId="9" r:id="rId8"/>
+    <sheet name="Oauth-mobile" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t xml:space="preserve">post a comment, and request comment detail </t>
   </si>
@@ -399,6 +400,45 @@
   </si>
   <si>
     <t>Offline discussion members does not receive discussion info changed notification</t>
+  </si>
+  <si>
+    <t>Oauth-login-bound-account</t>
+  </si>
+  <si>
+    <t>Oauth-login-bound-account-reg-new</t>
+  </si>
+  <si>
+    <t>User can request to log in via phone</t>
+  </si>
+  <si>
+    <t>Server returns vCode when requested (for first time)</t>
+  </si>
+  <si>
+    <t>Server returns error when vCode is invalid</t>
+  </si>
+  <si>
+    <t>Server let client login when vCode is valid and account is bound (previously)</t>
+  </si>
+  <si>
+    <t>Server requires client fill in registration form when vCode is valid, but account is not bound previously (new account reg via-phone)</t>
+  </si>
+  <si>
+    <t>Server let client login after client fill in registration form (valid) when register via phone number</t>
+  </si>
+  <si>
+    <t>User can log in without vCode if using the same deviceId as the previous ones</t>
+  </si>
+  <si>
+    <t>User cannot log in without vCode (server returns error) if using a new deviceId</t>
+  </si>
+  <si>
+    <t>User can request to log in via a second phone number</t>
+  </si>
+  <si>
+    <t>Server let user log in (using second phone number) if vCode is valid</t>
+  </si>
+  <si>
+    <t>User cannot login via phone (when phone number is unbound from his account)</t>
   </si>
 </sst>
 </file>
@@ -449,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -466,6 +506,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -809,7 +852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -828,14 +871,14 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1724,18 +1767,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -2418,14 +2461,14 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="2"/>
       <c r="I1" s="1"/>
     </row>
@@ -2968,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2980,18 +3023,18 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="3"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>104</v>
@@ -3298,4 +3341,320 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I15" si="0">SUM(B3:H3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SUM(B2:B15)</f>
+        <v>8</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" ref="C16:H16" si="1">SUM(C2:C15)</f>
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>